<commit_message>
Update issue 9 Status: Verified Documentación de las nuevas interfaces y uso de pines
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ordenes" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="163">
   <si>
     <t>Pin</t>
   </si>
@@ -485,13 +485,37 @@
   </si>
   <si>
     <t>No disponible</t>
+  </si>
+  <si>
+    <t>SolenoideOn</t>
+  </si>
+  <si>
+    <t>SolenoideOff</t>
+  </si>
+  <si>
+    <t>activarSolenoide3V()</t>
+  </si>
+  <si>
+    <t>desactivarSolenoide3V()</t>
+  </si>
+  <si>
+    <t>comprobarSolenoide3V()</t>
+  </si>
+  <si>
+    <t>0x67</t>
+  </si>
+  <si>
+    <t>0x68</t>
+  </si>
+  <si>
+    <t>0x69</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -532,6 +556,13 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -603,7 +634,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -663,8 +694,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -714,8 +747,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="61">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -745,6 +779,7 @@
     <cellStyle name="Hipervínculo" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -774,6 +809,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1106,7 +1142,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H13"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1415,23 +1451,53 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="E17" s="7"/>
-      <c r="F17" s="9"/>
-      <c r="H17" s="21" t="s">
+      <c r="A17" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F17" s="9">
+        <v>103</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>142</v>
       </c>
+      <c r="H17" s="14" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="E18" s="7"/>
-      <c r="F18" s="9"/>
-      <c r="H18" s="21" t="s">
+      <c r="A18" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F18" s="9">
+        <v>104</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>143</v>
       </c>
+      <c r="H18" s="14" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="E19" s="7"/>
-      <c r="F19" s="9"/>
-      <c r="H19" s="21" t="s">
+      <c r="A19" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" s="9">
+        <v>105</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1737,7 +1803,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1956,7 +2022,10 @@
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="C19" t="s">
+        <v>155</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1964,7 +2033,10 @@
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="C20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización del listado de pinas y órdenes de acuerdo a la especificación Sysreg 4.0
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16120" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ordenes" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="175">
   <si>
     <t>Pin</t>
   </si>
@@ -509,6 +509,42 @@
   </si>
   <si>
     <t>0x69</t>
+  </si>
+  <si>
+    <t>AlRegLAN</t>
+  </si>
+  <si>
+    <t>Ethernet Shield (SCK)</t>
+  </si>
+  <si>
+    <t>Ethernet Shield (MOSI)</t>
+  </si>
+  <si>
+    <t>Ethernet Shield (MISO)</t>
+  </si>
+  <si>
+    <t>Ethernet Shield (SS Ethernet)</t>
+  </si>
+  <si>
+    <t>Ethernet Shield (SS SD Card)</t>
+  </si>
+  <si>
+    <t>ICSP-4</t>
+  </si>
+  <si>
+    <t>ICSP-1</t>
+  </si>
+  <si>
+    <t>ICSP-3</t>
+  </si>
+  <si>
+    <t>I2C SDA (HR)</t>
+  </si>
+  <si>
+    <t>I2C SCL (HR)</t>
+  </si>
+  <si>
+    <t>Contador HW T1</t>
   </si>
 </sst>
 </file>
@@ -634,8 +670,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -735,6 +795,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -747,9 +808,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="85">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -780,6 +840,18 @@
     <cellStyle name="Hipervínculo" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -810,6 +882,18 @@
     <cellStyle name="Hipervínculo visitado" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1141,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1161,16 +1245,16 @@
       <c r="A1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4"/>
@@ -1451,7 +1535,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="23" t="s">
         <v>157</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -1468,7 +1552,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="23" t="s">
         <v>158</v>
       </c>
       <c r="E18" s="7" t="s">
@@ -1485,7 +1569,7 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="23" t="s">
         <v>159</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -1800,21 +1884,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="42.33203125" customWidth="1"/>
-    <col min="3" max="3" width="31.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3"/>
+    <col min="3" max="4" width="31.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1824,76 +1908,88 @@
       <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="D1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>151</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="E8" s="19" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1903,11 +1999,11 @@
       <c r="C9" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="E9" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1917,11 +2013,11 @@
       <c r="C10" t="s">
         <v>153</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="E10" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1931,11 +2027,11 @@
       <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="E11" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1945,11 +2041,11 @@
       <c r="C12" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="E12" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1959,88 +2055,109 @@
       <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="F14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="E18" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>155</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>156</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2050,11 +2167,14 @@
       <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2064,171 +2184,189 @@
       <c r="C22" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="E23" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="E24" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="E25" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="E26" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="E27" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="E28" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="E29" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="E30" s="19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="C31" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="E31" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="C32" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="E32" s="20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="C33" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="E33" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="C34" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="E34" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="E35" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="E36" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="C37" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="E37" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="C38" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="E38" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="E39" s="19" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="E40" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="E41" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="E42" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>